<commit_message>
fix : center-nowrap action
</commit_message>
<xml_diff>
--- a/public/excel/template_dosen.xlsx
+++ b/public/excel/template_dosen.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="22">
   <si>
     <t>Nama Dosen</t>
   </si>
@@ -29,9 +29,30 @@
     <t>NIP</t>
   </si>
   <si>
+    <t>Status (Aktif/Cuti/Resign/Pensiun)</t>
+  </si>
+  <si>
     <t>Nomor Telepon</t>
   </si>
   <si>
+    <t>Agama</t>
+  </si>
+  <si>
+    <t>Provinsi</t>
+  </si>
+  <si>
+    <t>Kota/Kabupaten</t>
+  </si>
+  <si>
+    <t>Kecamatan</t>
+  </si>
+  <si>
+    <t>Desa/Kelurahan</t>
+  </si>
+  <si>
+    <t>ID Program Studi</t>
+  </si>
+  <si>
     <t>Dosen Contoh</t>
   </si>
   <si>
@@ -41,7 +62,25 @@
     <t>L</t>
   </si>
   <si>
+    <t>Aktif</t>
+  </si>
+  <si>
     <t>081234567890</t>
+  </si>
+  <si>
+    <t>Islam</t>
+  </si>
+  <si>
+    <t>Jawa Barat</t>
+  </si>
+  <si>
+    <t>Bandung</t>
+  </si>
+  <si>
+    <t>Coblong</t>
+  </si>
+  <si>
+    <t>Dago</t>
   </si>
 </sst>
 </file>
@@ -397,10 +436,10 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="A1" sqref="A1:E1"/>
+      <selection activeCell="A1" sqref="A1:L1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -409,10 +448,17 @@
     <col min="2" max="2" width="17.567" bestFit="true" customWidth="true" style="0"/>
     <col min="3" max="3" width="23.423" bestFit="true" customWidth="true" style="0"/>
     <col min="4" max="4" width="22.28" bestFit="true" customWidth="true" style="0"/>
-    <col min="5" max="5" width="16.425" bestFit="true" customWidth="true" style="0"/>
+    <col min="5" max="5" width="41.133" bestFit="true" customWidth="true" style="0"/>
+    <col min="6" max="6" width="16.425" bestFit="true" customWidth="true" style="0"/>
+    <col min="7" max="7" width="6.998" bestFit="true" customWidth="true" style="0"/>
+    <col min="8" max="8" width="12.854" bestFit="true" customWidth="true" style="0"/>
+    <col min="9" max="9" width="17.567" bestFit="true" customWidth="true" style="0"/>
+    <col min="10" max="10" width="11.711" bestFit="true" customWidth="true" style="0"/>
+    <col min="11" max="11" width="17.567" bestFit="true" customWidth="true" style="0"/>
+    <col min="12" max="12" width="19.995" bestFit="true" customWidth="true" style="0"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:12">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -428,36 +474,69 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:12">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="C2" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="D2">
         <v>123456789012345678</v>
       </c>
       <c r="E2" t="s">
-        <v>8</v>
+        <v>15</v>
+      </c>
+      <c r="F2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H2" t="s">
+        <v>18</v>
+      </c>
+      <c r="I2" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2" t="s">
+        <v>20</v>
+      </c>
+      <c r="K2" t="s">
+        <v>21</v>
+      </c>
+      <c r="L2">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
   <printOptions gridLines="false" gridLinesSet="true"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="1" orientation="default" scale="100" fitToHeight="1" fitToWidth="1" pageOrder="downThenOver"/>
-  <headerFooter differentOddEven="false" differentFirst="false" scaleWithDoc="true" alignWithMargins="true">
-    <oddHeader/>
-    <oddFooter/>
-    <evenHeader/>
-    <evenFooter/>
-    <firstHeader/>
-    <firstFooter/>
-  </headerFooter>
-  <tableParts count="0"/>
 </worksheet>
 </file>
</xml_diff>